<commit_message>
cleanup index admin page
</commit_message>
<xml_diff>
--- a/docs/buglist.xlsx
+++ b/docs/buglist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>No</t>
   </si>
@@ -127,6 +127,36 @@
   <si>
     <t>belum ada halaman export data siswa ke excel</t>
   </si>
+  <si>
+    <t>Bisa kah default row in tablenya diganti 50?? -minor-</t>
+  </si>
+  <si>
+    <t>AUTH</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ketika admin keluar tanpa logout, maka ketika mengetikan </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">localhost, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">otomatis redirect to userpage</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -135,7 +165,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -175,6 +205,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -247,7 +284,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -282,6 +319,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -361,10 +402,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F1"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.4"/>
@@ -410,6 +451,7 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="B3" s="0"/>
       <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
@@ -424,6 +466,7 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="B4" s="0"/>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
@@ -438,6 +481,7 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="B5" s="0"/>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
@@ -455,6 +499,7 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="B6" s="0"/>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
@@ -469,6 +514,7 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="B7" s="0"/>
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
@@ -483,6 +529,7 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="B8" s="0"/>
       <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
@@ -497,6 +544,7 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="B9" s="0"/>
       <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
@@ -508,6 +556,7 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="B10" s="0"/>
       <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
@@ -519,12 +568,21 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
+      <c r="B11" s="0"/>
       <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
@@ -540,6 +598,7 @@
       <c r="A14" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="B14" s="0"/>
       <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
@@ -554,6 +613,7 @@
       <c r="A15" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="B15" s="0"/>
       <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
@@ -571,6 +631,7 @@
       <c r="A16" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="B16" s="0"/>
       <c r="C16" s="3" t="s">
         <v>24</v>
       </c>
@@ -582,7 +643,11 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="2"/>
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+      <c r="D17" s="0"/>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
@@ -607,6 +672,7 @@
       <c r="E19" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -653,11 +719,50 @@
         <v>9</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A13:F13"/>
     <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A25:F25"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
update bugfix, resolve missing lib and fix departement list
</commit_message>
<xml_diff>
--- a/docs/buglist.xlsx
+++ b/docs/buglist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
   <si>
     <t>No</t>
   </si>
@@ -35,7 +35,7 @@
     <t>applicant form</t>
   </si>
   <si>
-    <t>ketika sedang meingisi dan belum selesai, kemudia user klik tombol summary, maka harus redirect to hope page applicant, bukan halaman error</t>
+    <t>ketika sedang meingisi dan belum selesai, kemudia user klik tombol summary, maka harus redirect to home page applicant, bukan halaman error</t>
   </si>
   <si>
     <t>progress</t>
@@ -119,7 +119,28 @@
     <t>report per province</t>
   </si>
   <si>
-    <t>report per universities</t>
+    <r>
+      <t xml:space="preserve">report per universities(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF420E"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">dishow semua univ, utk filternya sementara menggunakan search</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t>belum ada halaman export data siswa ke excel</t>
@@ -165,7 +186,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -205,6 +226,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF420E"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -284,7 +312,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -319,6 +347,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -377,7 +409,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -401,7 +433,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.4"/>
@@ -412,7 +444,7 @@
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5714285714286"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -451,7 +483,6 @@
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -487,7 +518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
@@ -504,7 +535,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
@@ -534,7 +565,6 @@
       <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -546,8 +576,6 @@
       <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -559,8 +587,6 @@
       <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="0"/>
-      <c r="E10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -572,15 +598,10 @@
       <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="0"/>
-      <c r="E11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="B12" s="0"/>
-      <c r="C12" s="0"/>
-      <c r="D12" s="0"/>
-      <c r="E12" s="0"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
@@ -591,7 +612,7 @@
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>1</v>
       </c>
@@ -625,7 +646,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>3</v>
       </c>
@@ -643,11 +664,8 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
+      <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="0"/>
-      <c r="D17" s="0"/>
-      <c r="E17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
@@ -666,12 +684,11 @@
         <v>25</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -694,16 +711,18 @@
       <c r="A21" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>7</v>
+      <c r="C21" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="0"/>
+      <c r="E21" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -718,7 +737,6 @@
       <c r="D22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -733,7 +751,6 @@
       <c r="D23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -748,28 +765,18 @@
       <c r="D24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0"/>
-      <c r="B25" s="0"/>
-      <c r="C25" s="0"/>
-      <c r="D25" s="0"/>
-      <c r="E25" s="0"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
-      <c r="B26" s="0"/>
-      <c r="C26" s="0"/>
-      <c r="D26" s="0"/>
-      <c r="E26" s="0"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
-      <c r="B27" s="0"/>
-      <c r="C27" s="0"/>
-      <c r="D27" s="0"/>
-      <c r="E27" s="0"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
@@ -780,7 +787,7 @@
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
update buglist and add pesantren list
</commit_message>
<xml_diff>
--- a/docs/buglist.xlsx
+++ b/docs/buglist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="51" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="12" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="34">
   <si>
     <t>No</t>
   </si>
@@ -152,7 +152,7 @@
     <t>Bisa kah default row in tablenya diganti 50?? -minor-</t>
   </si>
   <si>
-    <t>fitur report berdasarkan pondok pesantren</t>
+    <t>fitur daftar pondok pesantren</t>
   </si>
   <si>
     <t>AUTH</t>
@@ -435,8 +435,8 @@
   </sheetPr>
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.4"/>
@@ -774,10 +774,13 @@
       <c r="B24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>15</v>
+      <c r="C24" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -802,10 +805,13 @@
       <c r="B26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>15</v>
+      <c r="C26" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -816,9 +822,6 @@
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="0"/>
-      <c r="D28" s="0"/>
-      <c r="E28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">

</xml_diff>